<commit_message>
n3xx: update PPS input constraint based on new cable prop delay calcs
</commit_message>
<xml_diff>
--- a/usrp3/top/n3xx/doc/mb_timing.xlsx
+++ b/usrp3/top/n3xx/doc/mb_timing.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\fpgadev\usrp3\top\n3xx\doc\"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="134">
   <si>
     <t>Delay Min</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>LMK00304</t>
+  </si>
+  <si>
+    <t>Cable Prop Delay</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -578,11 +581,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -625,17 +639,11 @@
     <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,10 +651,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -658,6 +672,8 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,12 +1431,12 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1532,22 +1548,22 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="H6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="40">
         <f>J5--I5</f>
         <v>6.8181381899999991</v>
       </c>
-      <c r="J6" s="35"/>
+      <c r="J6" s="36"/>
       <c r="K6" s="5" t="s">
         <v>45</v>
       </c>
@@ -1629,12 +1645,12 @@
       <c r="E9" s="17">
         <v>3.6</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1756,22 +1772,22 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
       <c r="H14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="42">
         <f>J13--I13</f>
         <v>3.7421314300000001</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="36"/>
       <c r="K14" s="21" t="s">
         <v>45</v>
       </c>
@@ -1951,23 +1967,23 @@
       <c r="I22" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
@@ -2034,14 +2050,14 @@
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
@@ -2252,16 +2268,16 @@
       <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -2353,7 +2369,7 @@
       <c r="K4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -2387,7 +2403,7 @@
       </c>
       <c r="L5" s="12">
         <f>B4-C30</f>
-        <v>38.885260000000002</v>
+        <v>38.765259999999998</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>40</v>
@@ -2417,7 +2433,7 @@
       </c>
       <c r="L6" s="12">
         <f>C49</f>
-        <v>5.0608599999999999</v>
+        <v>5.1808600000000009</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2453,7 +2469,7 @@
       </c>
       <c r="L7" s="10">
         <f>C30</f>
-        <v>1.1147399999999994</v>
+        <v>1.2347399999999995</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>63</v>
@@ -2491,7 +2507,7 @@
       </c>
       <c r="L8" s="10">
         <f>C49</f>
-        <v>5.0608599999999999</v>
+        <v>5.1808600000000009</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>69</v>
@@ -2539,15 +2555,23 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="47">
+        <v>0.122</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2585,12 +2609,12 @@
         <v>88</v>
       </c>
       <c r="B16" s="17">
-        <f>B9*B3</f>
-        <v>2.04</v>
+        <f>B9*B11</f>
+        <v>1.464</v>
       </c>
       <c r="C16" s="16">
         <f t="shared" ref="C16:C19" si="4">C15+B16</f>
-        <v>-2.96</v>
+        <v>-3.536</v>
       </c>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
@@ -2605,7 +2629,7 @@
       </c>
       <c r="C17" s="16">
         <f t="shared" si="4"/>
-        <v>-2.8976099999999998</v>
+        <v>-3.4736099999999999</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
@@ -2619,7 +2643,7 @@
       </c>
       <c r="C18" s="16">
         <f t="shared" si="4"/>
-        <v>0.70239000000000029</v>
+        <v>0.12639000000000022</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>71</v>
@@ -2635,7 +2659,7 @@
       </c>
       <c r="C19" s="16">
         <f t="shared" si="4"/>
-        <v>1.4053400000000003</v>
+        <v>0.8293400000000003</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2646,7 +2670,7 @@
       <c r="B20" s="16"/>
       <c r="C20" s="23">
         <f>C19</f>
-        <v>1.4053400000000003</v>
+        <v>0.8293400000000003</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2687,12 +2711,12 @@
         <v>88</v>
       </c>
       <c r="B24" s="17">
-        <f>B9*B2</f>
-        <v>1.92</v>
+        <f>B9*B11</f>
+        <v>1.464</v>
       </c>
       <c r="C24" s="16">
         <f t="shared" ref="C24:C28" si="5">C23+B24</f>
-        <v>1.92</v>
+        <v>1.464</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2706,7 +2730,7 @@
       </c>
       <c r="C25" s="16">
         <f t="shared" si="5"/>
-        <v>2.1228799999999999</v>
+        <v>1.6668799999999999</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2720,7 +2744,7 @@
       </c>
       <c r="C26" s="16">
         <f t="shared" si="5"/>
-        <v>2.2928799999999998</v>
+        <v>1.8368799999999998</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>99</v>
@@ -2736,7 +2760,7 @@
       </c>
       <c r="C27" s="16">
         <f t="shared" si="5"/>
-        <v>2.7200799999999998</v>
+        <v>2.2640799999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2749,7 +2773,7 @@
       </c>
       <c r="C28" s="16">
         <f t="shared" si="5"/>
-        <v>2.5200799999999997</v>
+        <v>2.0640799999999997</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2759,7 +2783,7 @@
       <c r="B29" s="3"/>
       <c r="C29" s="23">
         <f>C28</f>
-        <v>2.5200799999999997</v>
+        <v>2.0640799999999997</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2769,7 +2793,7 @@
       <c r="B30" s="26"/>
       <c r="C30" s="23">
         <f>C29-C20</f>
-        <v>1.1147399999999994</v>
+        <v>1.2347399999999995</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>102</v>
@@ -2782,9 +2806,9 @@
       <c r="A32" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
@@ -2820,12 +2844,12 @@
         <v>88</v>
       </c>
       <c r="B35" s="17">
-        <f>B9*B2</f>
-        <v>1.92</v>
+        <f>B9*B11</f>
+        <v>1.464</v>
       </c>
       <c r="C35" s="16">
         <f t="shared" ref="C35:C38" si="6">C34+B35</f>
-        <v>6.92</v>
+        <v>6.4640000000000004</v>
       </c>
       <c r="D35" s="1"/>
     </row>
@@ -2839,7 +2863,7 @@
       </c>
       <c r="C36" s="16">
         <f t="shared" si="6"/>
-        <v>6.97872</v>
+        <v>6.5227200000000005</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -2853,7 +2877,7 @@
       </c>
       <c r="C37" s="16">
         <f t="shared" si="6"/>
-        <v>7.6787200000000002</v>
+        <v>7.2227200000000007</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>71</v>
@@ -2869,7 +2893,7 @@
       </c>
       <c r="C38" s="16">
         <f t="shared" si="6"/>
-        <v>8.3403200000000002</v>
+        <v>7.8843200000000007</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -2880,7 +2904,7 @@
       <c r="B39" s="16"/>
       <c r="C39" s="23">
         <f>C38</f>
-        <v>8.3403200000000002</v>
+        <v>7.8843200000000007</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2920,12 +2944,12 @@
         <v>88</v>
       </c>
       <c r="B43" s="16">
-        <f>B9*B3</f>
-        <v>2.04</v>
+        <f>B9*B11</f>
+        <v>1.464</v>
       </c>
       <c r="C43" s="16">
         <f t="shared" ref="C43:C47" si="7">C42+B43</f>
-        <v>2.04</v>
+        <v>1.464</v>
       </c>
       <c r="D43" s="1"/>
     </row>
@@ -2939,7 +2963,7 @@
       </c>
       <c r="C44" s="16">
         <f t="shared" si="7"/>
-        <v>2.25556</v>
+        <v>1.6795599999999999</v>
       </c>
       <c r="D44" s="1"/>
     </row>
@@ -2952,7 +2976,7 @@
       </c>
       <c r="C45" s="16">
         <f t="shared" si="7"/>
-        <v>2.6255600000000001</v>
+        <v>2.04956</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>99</v>
@@ -2968,7 +2992,7 @@
       </c>
       <c r="C46" s="16">
         <f t="shared" si="7"/>
-        <v>3.0794600000000001</v>
+        <v>2.50346</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2981,7 +3005,7 @@
       </c>
       <c r="C47" s="16">
         <f t="shared" si="7"/>
-        <v>3.2794600000000003</v>
+        <v>2.7034600000000002</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2991,7 +3015,7 @@
       <c r="B48" s="3"/>
       <c r="C48" s="23">
         <f>C47</f>
-        <v>3.2794600000000003</v>
+        <v>2.7034600000000002</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -3001,7 +3025,7 @@
       <c r="B49" s="26"/>
       <c r="C49" s="23">
         <f>C39-C48</f>
-        <v>5.0608599999999999</v>
+        <v>5.1808600000000009</v>
       </c>
       <c r="D49" s="27" t="s">
         <v>113</v>
@@ -5922,16 +5946,16 @@
       <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -6023,7 +6047,7 @@
       <c r="K4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -6198,9 +6222,9 @@
       <c r="A13" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
@@ -6377,9 +6401,9 @@
       <c r="A28" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">

</xml_diff>

<commit_message>
n3xx: update PPS input timing parameters for SN74LVC2G34 buffer
Constraints are backwards compatible with old and new devices.
</commit_message>
<xml_diff>
--- a/usrp3/top/n3xx/doc/mb_timing.xlsx
+++ b/usrp3/top/n3xx/doc/mb_timing.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\fpgadev\usrp3\top\n3xx\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A539DA92-3817-45EE-BA67-1B503600CDF3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of PPS Timing Closure" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Ext PPS Capture" sheetId="2" r:id="rId2"/>
     <sheet name="GPS PPS Capture" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="135">
   <si>
     <t>Delay Min</t>
   </si>
@@ -423,12 +424,15 @@
   </si>
   <si>
     <t>Cable Prop Delay</t>
+  </si>
+  <si>
+    <t>SN74LVC @ 3.3V, 30 pF Capacitive load</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -639,6 +643,8 @@
     <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -672,8 +678,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,7 +1404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1431,12 +1435,12 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1548,22 +1552,22 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="H6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="42">
         <f>J5--I5</f>
         <v>6.8181381899999991</v>
       </c>
-      <c r="J6" s="36"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="5" t="s">
         <v>45</v>
       </c>
@@ -1645,12 +1649,12 @@
       <c r="E9" s="17">
         <v>3.6</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1772,22 +1776,22 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
       <c r="H14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="44">
         <f>J13--I13</f>
         <v>3.7421314300000001</v>
       </c>
-      <c r="J14" s="36"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="21" t="s">
         <v>45</v>
       </c>
@@ -1967,23 +1971,23 @@
       <c r="I22" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="43"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
@@ -2050,14 +2054,14 @@
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
@@ -2241,12 +2245,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2265,19 +2269,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -2366,10 +2370,10 @@
         <f t="shared" si="1"/>
         <v>5.2700000000000004E-3</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="36"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -2403,7 +2407,7 @@
       </c>
       <c r="L5" s="12">
         <f>B4-C30</f>
-        <v>38.765259999999998</v>
+        <v>39.765259999999998</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>40</v>
@@ -2433,7 +2437,7 @@
       </c>
       <c r="L6" s="12">
         <f>C49</f>
-        <v>5.1808600000000009</v>
+        <v>4.6508599999999998</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,7 +2473,7 @@
       </c>
       <c r="L7" s="10">
         <f>C30</f>
-        <v>1.2347399999999995</v>
+        <v>0.23473999999999995</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>63</v>
@@ -2507,7 +2511,7 @@
       </c>
       <c r="L8" s="10">
         <f>C49</f>
-        <v>5.1808600000000009</v>
+        <v>4.6508599999999998</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>69</v>
@@ -2558,20 +2562,20 @@
       <c r="A11" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="34">
         <v>0.122</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2639,14 +2643,14 @@
         <v>96</v>
       </c>
       <c r="B18" s="17">
-        <v>3.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C18" s="16">
         <f t="shared" si="4"/>
-        <v>0.12639000000000022</v>
+        <v>1.1263899999999998</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2659,7 +2663,7 @@
       </c>
       <c r="C19" s="16">
         <f t="shared" si="4"/>
-        <v>0.8293400000000003</v>
+        <v>1.8293399999999997</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2670,7 +2674,7 @@
       <c r="B20" s="16"/>
       <c r="C20" s="23">
         <f>C19</f>
-        <v>0.8293400000000003</v>
+        <v>1.8293399999999997</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2793,7 +2797,7 @@
       <c r="B30" s="26"/>
       <c r="C30" s="23">
         <f>C29-C20</f>
-        <v>1.2347399999999995</v>
+        <v>0.23473999999999995</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>102</v>
@@ -2803,12 +2807,12 @@
       <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
@@ -2872,15 +2876,14 @@
         <v>96</v>
       </c>
       <c r="B37" s="16">
-        <f>0.7</f>
-        <v>0.7</v>
+        <v>0.17</v>
       </c>
       <c r="C37" s="16">
         <f t="shared" si="6"/>
-        <v>7.2227200000000007</v>
+        <v>6.6927200000000004</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2896,7 @@
       </c>
       <c r="C38" s="16">
         <f t="shared" si="6"/>
-        <v>7.8843200000000007</v>
+        <v>7.3543200000000004</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -2904,7 +2907,7 @@
       <c r="B39" s="16"/>
       <c r="C39" s="23">
         <f>C38</f>
-        <v>7.8843200000000007</v>
+        <v>7.3543200000000004</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3025,7 +3028,7 @@
       <c r="B49" s="26"/>
       <c r="C49" s="23">
         <f>C39-C48</f>
-        <v>5.1808600000000009</v>
+        <v>4.6508599999999998</v>
       </c>
       <c r="D49" s="27" t="s">
         <v>113</v>
@@ -5919,7 +5922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5943,19 +5946,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -6044,10 +6047,10 @@
         <f t="shared" si="1"/>
         <v>0.38386000000000003</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="36"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -6219,12 +6222,12 @@
       <c r="A11" s="3"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
@@ -6398,12 +6401,12 @@
       <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">

</xml_diff>